<commit_message>
114059 - CBA Cost Calc.
</commit_message>
<xml_diff>
--- a/114059 - Estimation/Excercise/CostBenefitAnalysis.xlsx
+++ b/114059 - Estimation/Excercise/CostBenefitAnalysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\LearnershipSecondBlock\114059 - Estimation\Excercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3748DE73-EF40-4A5A-A49B-FA70897F5119}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD15FCD-8FB9-478B-A720-06396DA2DE42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{E7F094A6-971F-4ADA-8429-34669171EE37}"/>
   </bookViews>
@@ -17,6 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="PERT_Expected">Sheet1!$E$15</definedName>
+    <definedName name="Rate_Per_Hour">Sheet1!$K$14</definedName>
     <definedName name="Std_Deviation">Sheet1!$G$15</definedName>
     <definedName name="StdDeviationValue">Sheet1!$H$15</definedName>
   </definedNames>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>User Stories</t>
   </si>
@@ -141,12 +142,18 @@
   </si>
   <si>
     <t>Std Dev Percent</t>
+  </si>
+  <si>
+    <t>Rate Per Hour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="&quot;R&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -249,7 +256,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -258,24 +265,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="3" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
@@ -301,19 +316,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <top style="thick">
+          <color theme="4" tint="0.499984740745262"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -341,11 +348,22 @@
       </font>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thick">
-          <color theme="4" tint="0.499984740745262"/>
-        </top>
-      </border>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -365,9 +383,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -382,20 +397,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A9E4A43B-4DC1-4428-85B1-19796372DE36}" name="UserStories" displayName="UserStories" ref="A2:H13" totalsRowCount="1" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A9E4A43B-4DC1-4428-85B1-19796372DE36}" name="UserStories" displayName="UserStories" ref="A2:H13" totalsRowCount="1" headerRowDxfId="13">
   <autoFilter ref="A2:H12" xr:uid="{083DA0AD-1B03-4972-9CD2-3F69AC7C36B8}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{2E9BC4ED-5A86-4643-94E8-38AFD9FB0D73}" name="Ref" totalsRowLabel="Total" totalsRowCellStyle="60% - Accent6"/>
-    <tableColumn id="2" xr3:uid="{DA8A69A4-2AFA-434F-A9BE-B47AA35DA813}" name="Story" dataDxfId="13" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{DA8A69A4-2AFA-434F-A9BE-B47AA35DA813}" name="Story" dataDxfId="12" totalsRowDxfId="11"/>
     <tableColumn id="4" xr3:uid="{DBB2D4FE-F8BA-444A-ACB1-63E8CDE355C9}" name="Size "/>
     <tableColumn id="5" xr3:uid="{81D412DB-B867-4BEF-8E8D-D56BB9F4AA7B}" name="Complexity"/>
-    <tableColumn id="6" xr3:uid="{F638A209-87D6-4342-87B8-E866FC6FED01}" name="Optimistic" totalsRowFunction="sum" dataDxfId="6" totalsRowCellStyle="60% - Accent6">
+    <tableColumn id="6" xr3:uid="{F638A209-87D6-4342-87B8-E866FC6FED01}" name="Optimistic" totalsRowFunction="sum" dataDxfId="10" totalsRowCellStyle="60% - Accent6">
       <calculatedColumnFormula>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],2,FALSE)*UserStories[[#This Row],[Factor]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{044D33E7-4199-4287-AEB5-010BED4820FE}" name="Expected" totalsRowFunction="sum" dataDxfId="5" totalsRowCellStyle="60% - Accent6">
+    <tableColumn id="7" xr3:uid="{044D33E7-4199-4287-AEB5-010BED4820FE}" name="Expected" totalsRowFunction="sum" dataDxfId="9" totalsRowCellStyle="60% - Accent6">
       <calculatedColumnFormula>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],3,FALSE)*UserStories[[#This Row],[Factor]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E397F8BA-9C70-4E8E-B2D4-F85221571C8F}" name="Persimistic" totalsRowFunction="sum" dataDxfId="4" totalsRowCellStyle="60% - Accent6">
+    <tableColumn id="8" xr3:uid="{E397F8BA-9C70-4E8E-B2D4-F85221571C8F}" name="Persimistic" totalsRowFunction="sum" dataDxfId="8" totalsRowCellStyle="60% - Accent6">
       <calculatedColumnFormula>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],4,FALSE)*UserStories[[#This Row],[Factor]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{3C0F2416-ADCE-45CC-A332-5C814B3167FA}" name="Factor" totalsRowFunction="sum" dataDxfId="7" totalsRowCellStyle="60% - Accent6">
@@ -407,7 +422,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6BAB53AE-A8E4-4968-B4DB-EC442C0B86A5}" name="SizeEstimations" displayName="SizeEstimations" ref="A23:D26" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6BAB53AE-A8E4-4968-B4DB-EC442C0B86A5}" name="SizeEstimations" displayName="SizeEstimations" ref="A23:D26" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A23:D26" xr:uid="{0DF855A2-DFAC-4B88-9323-E75A0F23483E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{991B154E-750E-4DD5-97A8-4A5A1AC48BB3}" name="Size "/>
@@ -420,10 +435,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E353E001-C031-4257-8F70-DA6C7C1C275B}" name="ComplexityEstimations" displayName="ComplexityEstimations" ref="A30:B33" totalsRowShown="0" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E353E001-C031-4257-8F70-DA6C7C1C275B}" name="ComplexityEstimations" displayName="ComplexityEstimations" ref="A30:B33" totalsRowShown="0" tableBorderDxfId="4">
   <autoFilter ref="A30:B33" xr:uid="{FA2C4184-1F49-4770-A24D-33B51BC28BFB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D8584182-7C90-4FBF-B162-66C392D34A40}" name="Complexity" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{D8584182-7C90-4FBF-B162-66C392D34A40}" name="Complexity" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{D9F73F0D-134B-40ED-8FC3-EFE8CCB98D40}" name="Factor"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -739,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28518105-A2B1-46B8-BB45-D4A179BC2835}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,17 +770,18 @@
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -791,7 +807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -816,12 +832,12 @@
         <f>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],4,FALSE)*UserStories[[#This Row],[Factor]]</f>
         <v>18</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Complexity]],ComplexityEstimations[],2,FALSE)</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -846,12 +862,12 @@
         <f>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],4,FALSE)*UserStories[[#This Row],[Factor]]</f>
         <v>18</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Complexity]],ComplexityEstimations[],2,FALSE)</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -876,12 +892,12 @@
         <f>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],4,FALSE)*UserStories[[#This Row],[Factor]]</f>
         <v>9</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Complexity]],ComplexityEstimations[],2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -906,12 +922,12 @@
         <f>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],4,FALSE)*UserStories[[#This Row],[Factor]]</f>
         <v>9</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Complexity]],ComplexityEstimations[],2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -924,24 +940,24 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],2,FALSE)*UserStories[[#This Row],[Factor]]</f>
         <v>1.35</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],3,FALSE)*UserStories[[#This Row],[Factor]]</f>
         <v>2.7</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],4,FALSE)*UserStories[[#This Row],[Factor]]</f>
         <v>5.4</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Complexity]],ComplexityEstimations[],2,FALSE)</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -966,12 +982,12 @@
         <f>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],4,FALSE)*UserStories[[#This Row],[Factor]]</f>
         <v>9</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Complexity]],ComplexityEstimations[],2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -996,12 +1012,12 @@
         <f>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],4,FALSE)*UserStories[[#This Row],[Factor]]</f>
         <v>5.4</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Complexity]],ComplexityEstimations[],2,FALSE)</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1026,12 +1042,12 @@
         <f>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],4,FALSE)*UserStories[[#This Row],[Factor]]</f>
         <v>6</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Complexity]],ComplexityEstimations[],2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1056,12 +1072,12 @@
         <f>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],4,FALSE)*UserStories[[#This Row],[Factor]]</f>
         <v>5.4</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Complexity]],ComplexityEstimations[],2,FALSE)</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1086,66 +1102,85 @@
         <f>VLOOKUP(UserStories[[#This Row],[Size ]],SizeEstimations[],4,FALSE)*UserStories[[#This Row],[Factor]]</f>
         <v>5.4</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="4">
         <f>VLOOKUP(UserStories[[#This Row],[Complexity]],ComplexityEstimations[],2,FALSE)</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <f>SUBTOTAL(109,UserStories[Optimistic])</f>
         <v>33.900000000000006</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <f>SUBTOTAL(109,UserStories[Expected])</f>
         <v>58.800000000000011</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="7">
         <f>SUBTOTAL(109,UserStories[Persimistic])</f>
         <v>90.600000000000023</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="7">
         <f>SUBTOTAL(109,UserStories[Factor])</f>
         <v>10.600000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="7">
         <f>(UserStories[[#Totals],[Optimistic]]+(4*UserStories[[#Totals],[Expected]])+UserStories[[#Totals],[Persimistic]])/6</f>
         <v>59.95000000000001</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="14">
         <v>0.5</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <f>(UserStories[[#Totals],[Persimistic]] - UserStories[[#Totals],[Optimistic]])/6</f>
         <v>9.4500000000000028</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15" s="1"/>
+      <c r="K15" s="17">
+        <f>Rate_Per_Hour*PERT_Expected</f>
+        <v>5995.0000000000009</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="17"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>0.5</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="10">
         <f>PERT_Expected+D16*StdDeviationValue</f>
         <v>64.675000000000011</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="9">
         <f>F15+VLOOKUP(D16,StdDeviation[],2,FALSE)</f>
         <v>0.69100000000000006</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K16" s="13">
+        <f>Rate_Per_Hour*E16</f>
+        <v>6467.5000000000009</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>1</v>
       </c>
@@ -1153,59 +1188,75 @@
         <f>PERT_Expected+D17*StdDeviationValue</f>
         <v>69.400000000000006</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="9">
         <f>F16+VLOOKUP(D17,StdDeviation[],2,FALSE)</f>
         <v>0.84100000000000008</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K17" s="13">
+        <f>Rate_Per_Hour*E17</f>
+        <v>6940.0000000000009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>1.5</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="15">
         <f>PERT_Expected+D18*StdDeviationValue</f>
         <v>74.125000000000014</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="16">
         <f>F17+VLOOKUP(D18,StdDeviation[],2,FALSE)</f>
         <v>0.93300000000000005</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K18" s="13">
+        <f>Rate_Per_Hour*E18</f>
+        <v>7412.5000000000018</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>2</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="10">
         <f>PERT_Expected+D19*StdDeviationValue</f>
         <v>78.850000000000023</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="9">
         <f>F18+VLOOKUP(D19,StdDeviation[],2,FALSE)</f>
         <v>0.97700000000000009</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K19" s="13">
+        <f>Rate_Per_Hour*E19</f>
+        <v>7885.0000000000018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>2.5</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="10">
         <f>PERT_Expected+D20*StdDeviationValue</f>
         <v>83.575000000000017</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="9">
         <f>F19+VLOOKUP(D20,StdDeviation[],2,FALSE)</f>
         <v>0.99400000000000011</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
+      <c r="K20" s="13">
+        <f>Rate_Per_Hour*E20</f>
+        <v>8357.5000000000018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -1219,7 +1270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1233,7 +1284,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1247,7 +1298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1261,13 +1312,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="11"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
@@ -1275,7 +1326,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
@@ -1283,7 +1334,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>9</v>
       </c>
@@ -1300,11 +1351,11 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1321,10 +1372,10 @@
       <c r="A38">
         <v>0.5</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="5">
         <v>0.191</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="5">
         <v>0.191</v>
       </c>
     </row>
@@ -1332,10 +1383,10 @@
       <c r="A39">
         <v>1</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="6">
         <v>0.15</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="5">
         <v>0.34100000000000003</v>
       </c>
     </row>
@@ -1343,10 +1394,10 @@
       <c r="A40">
         <v>1.5</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="5">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="5">
         <v>0.433</v>
       </c>
     </row>
@@ -1354,10 +1405,10 @@
       <c r="A41">
         <v>2</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="5">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="5">
         <v>0.47699999999999998</v>
       </c>
     </row>
@@ -1365,10 +1416,10 @@
       <c r="A42">
         <v>2.5</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="5">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="5">
         <v>0.49399999999999999</v>
       </c>
     </row>
@@ -1376,10 +1427,10 @@
       <c r="A43">
         <v>3</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="5">
         <v>0.499</v>
       </c>
     </row>
@@ -1391,11 +1442,12 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="4">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>